<commit_message>
Added results of GGZ with run length.
</commit_message>
<xml_diff>
--- a/Resuts/result.xlsx
+++ b/Resuts/result.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Filename</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>LZ77txt</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>GGZRLE</t>
   </si>
 </sst>
 </file>
@@ -734,7 +740,848 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="70">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -1024,18 +1871,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S47" sqref="S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1066,8 +1915,14 @@
       <c r="J1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="K1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1098,8 +1953,15 @@
       <c r="J2">
         <v>14260</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="K2">
+        <v>12802</v>
+      </c>
+      <c r="N2">
+        <f>SMALL(B2:K2,1)</f>
+        <v>12802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1130,8 +1992,15 @@
       <c r="J3">
         <v>365690</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="K3">
+        <v>266946</v>
+      </c>
+      <c r="N3">
+        <f>SMALL(B3:K3,1)</f>
+        <v>251157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1162,8 +2031,15 @@
       <c r="J4">
         <v>9980</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="K4">
+        <v>8932</v>
+      </c>
+      <c r="N4">
+        <f>SMALL(B4:K4,1)</f>
+        <v>8932</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1194,8 +2070,15 @@
       <c r="J5">
         <v>227106</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="K5">
+        <v>167429</v>
+      </c>
+      <c r="N5">
+        <f>SMALL(B5:K5,1)</f>
+        <v>160328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1226,8 +2109,15 @@
       <c r="J6">
         <v>51004</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="K6">
+        <v>41241</v>
+      </c>
+      <c r="N6">
+        <f>SMALL(B6:K6,1)</f>
+        <v>41241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1258,8 +2148,15 @@
       <c r="J7">
         <v>210611</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="K7">
+        <v>173420</v>
+      </c>
+      <c r="N7">
+        <f>SMALL(B7:K7,1)</f>
+        <v>146200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1290,8 +2187,15 @@
       <c r="J8">
         <v>493472</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="K8">
+        <v>393296</v>
+      </c>
+      <c r="N8">
+        <f>SMALL(B8:K8,1)</f>
+        <v>353514</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1322,9 +2226,16 @@
       <c r="J9">
         <v>14571</v>
       </c>
+      <c r="K9">
+        <v>14527</v>
+      </c>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9">
+        <f>SMALL(B9:K9,1)</f>
+        <v>14527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1355,8 +2266,15 @@
       <c r="J10">
         <v>171562</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="K10">
+        <v>127720</v>
+      </c>
+      <c r="N10">
+        <f>SMALL(B10:K10,1)</f>
+        <v>119182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1387,8 +2305,15 @@
       <c r="J11">
         <v>238616</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="K11">
+        <v>179129</v>
+      </c>
+      <c r="N11">
+        <f>SMALL(B11:K11,1)</f>
+        <v>167626</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1419,8 +2344,15 @@
       <c r="J12">
         <v>93379</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="K12">
+        <v>77909</v>
+      </c>
+      <c r="N12">
+        <f>SMALL(B12:K12,1)</f>
+        <v>72718</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1451,8 +2383,15 @@
       <c r="J13">
         <v>146378</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="K13">
+        <v>108878</v>
+      </c>
+      <c r="N13">
+        <f>SMALL(B13:K13,1)</f>
+        <v>101945</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1483,8 +2422,15 @@
       <c r="J14">
         <v>198818</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="K14">
+        <v>129331</v>
+      </c>
+      <c r="N14">
+        <f>SMALL(B14:K14,1)</f>
+        <v>129331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1515,8 +2461,15 @@
       <c r="J15">
         <v>27498</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="K15">
+        <v>22786</v>
+      </c>
+      <c r="N15">
+        <f>SMALL(B15:K15,1)</f>
+        <v>21896</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1547,8 +2500,15 @@
       <c r="J16">
         <v>206711</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <v>153400</v>
+      </c>
+      <c r="N16">
+        <f>SMALL(B16:K16,1)</f>
+        <v>142748</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1579,8 +2539,15 @@
       <c r="J17">
         <v>290686</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <v>210992</v>
+      </c>
+      <c r="N17">
+        <f>SMALL(B17:K17,1)</f>
+        <v>210992</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1611,8 +2578,15 @@
       <c r="J18">
         <v>346067</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>250200</v>
+      </c>
+      <c r="N18">
+        <f>SMALL(B18:K18,1)</f>
+        <v>250200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1643,8 +2617,15 @@
       <c r="J19">
         <v>214346</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19">
+        <v>196090</v>
+      </c>
+      <c r="N19">
+        <f>SMALL(B19:K19,1)</f>
+        <v>163036</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1675,8 +2656,15 @@
       <c r="J20">
         <v>854938</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>784745</v>
+      </c>
+      <c r="N20">
+        <f>SMALL(B20:K20,1)</f>
+        <v>663477</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1707,8 +2695,15 @@
       <c r="J21">
         <v>70637</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>65428</v>
+      </c>
+      <c r="N21">
+        <f>SMALL(B21:K21,1)</f>
+        <v>52236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1739,8 +2734,15 @@
       <c r="J22">
         <v>272466</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <v>231366</v>
+      </c>
+      <c r="N22">
+        <f>SMALL(B22:K22,1)</f>
+        <v>183402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1771,8 +2773,15 @@
       <c r="J23">
         <v>84276</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <v>62966</v>
+      </c>
+      <c r="N23">
+        <f>SMALL(B23:K23,1)</f>
+        <v>59928</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1803,8 +2812,15 @@
       <c r="J24">
         <v>274272</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <v>244824</v>
+      </c>
+      <c r="N24">
+        <f>SMALL(B24:K24,1)</f>
+        <v>192368</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1835,8 +2851,15 @@
       <c r="J25">
         <v>631634</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <v>458717</v>
+      </c>
+      <c r="N25">
+        <f>SMALL(B25:K25,1)</f>
+        <v>411412</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1867,8 +2890,15 @@
       <c r="J26">
         <v>136830</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26">
+        <v>100494</v>
+      </c>
+      <c r="N26">
+        <f>SMALL(B26:K26,1)</f>
+        <v>95446</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1899,8 +2929,15 @@
       <c r="J27">
         <v>1783</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27">
+        <v>3411</v>
+      </c>
+      <c r="N27">
+        <f>SMALL(B27:K27,1)</f>
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1931,8 +2968,15 @@
       <c r="J28">
         <v>12642</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28">
+        <v>11542</v>
+      </c>
+      <c r="N28">
+        <f>SMALL(B28:K28,1)</f>
+        <v>10530</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1963,8 +3007,15 @@
       <c r="J29">
         <v>2425</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29">
+        <v>3740</v>
+      </c>
+      <c r="N29">
+        <f>SMALL(B29:K29,1)</f>
+        <v>2151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1995,8 +3046,15 @@
       <c r="J30">
         <v>804172</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30">
+        <v>639672</v>
+      </c>
+      <c r="N30">
+        <f>SMALL(B30:K30,1)</f>
+        <v>580327</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2027,8 +3085,15 @@
       <c r="J31">
         <v>283084</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31">
+        <v>251310</v>
+      </c>
+      <c r="N31">
+        <f>SMALL(B31:K31,1)</f>
+        <v>202451</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2059,8 +3124,15 @@
       <c r="J32">
         <v>218404</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32">
+        <v>181679</v>
+      </c>
+      <c r="N32">
+        <f>SMALL(B32:K32,1)</f>
+        <v>168170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2091,8 +3163,15 @@
       <c r="J33">
         <v>210461</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33">
+        <v>152334</v>
+      </c>
+      <c r="N33">
+        <f>SMALL(B33:K33,1)</f>
+        <v>147295</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2123,8 +3202,15 @@
       <c r="J34">
         <v>14032</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34">
+        <v>14874</v>
+      </c>
+      <c r="N34">
+        <f>SMALL(B34:K34,1)</f>
+        <v>13430</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2155,8 +3241,15 @@
       <c r="J35">
         <v>112086</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35">
+        <v>101893</v>
+      </c>
+      <c r="N35">
+        <f>SMALL(B35:K35,1)</f>
+        <v>93701</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2187,8 +3280,15 @@
       <c r="J36">
         <v>29153</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36">
+        <v>23025</v>
+      </c>
+      <c r="N36">
+        <f>SMALL(B36:K36,1)</f>
+        <v>22346</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2219,8 +3319,15 @@
       <c r="J37">
         <v>46820</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37">
+        <v>35822</v>
+      </c>
+      <c r="N37">
+        <f>SMALL(B37:K37,1)</f>
+        <v>34370</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2251,8 +3358,15 @@
       <c r="J38">
         <v>242113</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38">
+        <v>159881</v>
+      </c>
+      <c r="N38">
+        <f>SMALL(B38:K38,1)</f>
+        <v>159881</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2283,8 +3397,15 @@
       <c r="J39">
         <v>224123</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39">
+        <v>151788</v>
+      </c>
+      <c r="N39">
+        <f>SMALL(B39:K39,1)</f>
+        <v>151788</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2315,8 +3436,15 @@
       <c r="J40">
         <v>74595</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40">
+        <v>65902</v>
+      </c>
+      <c r="N40">
+        <f>SMALL(B40:K40,1)</f>
+        <v>65902</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2347,8 +3475,15 @@
       <c r="J41">
         <v>272289</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41">
+        <v>240145</v>
+      </c>
+      <c r="N41">
+        <f>SMALL(B41:K41,1)</f>
+        <v>190131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2379,8 +3514,15 @@
       <c r="J42">
         <v>1981475</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="K42">
+        <v>1434082</v>
+      </c>
+      <c r="N42">
+        <f>SMALL(B42:K42,1)</f>
+        <v>1378371</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2411,8 +3553,15 @@
       <c r="J43">
         <v>20860</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="K43">
+        <v>17735</v>
+      </c>
+      <c r="N43">
+        <f>SMALL(B43:K43,1)</f>
+        <v>16772</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2443,8 +3592,15 @@
       <c r="J44">
         <v>25220</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="K44">
+        <v>22717</v>
+      </c>
+      <c r="N44">
+        <f>SMALL(B44:K44,1)</f>
+        <v>21233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2475,8 +3631,15 @@
       <c r="J45">
         <v>17585</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45">
+        <v>15641</v>
+      </c>
+      <c r="N45">
+        <f>SMALL(B45:K45,1)</f>
+        <v>14820</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2507,8 +3670,15 @@
       <c r="J46">
         <v>9308</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="K46">
+        <v>9186</v>
+      </c>
+      <c r="N46">
+        <f>SMALL(B46:K46,1)</f>
+        <v>9186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2539,8 +3709,15 @@
       <c r="J47">
         <v>166924</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="K47">
+        <v>124575</v>
+      </c>
+      <c r="N47">
+        <f>SMALL(B47:K47,1)</f>
+        <v>115899</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2571,8 +3748,15 @@
       <c r="J48">
         <v>15204</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="K48">
+        <v>10571</v>
+      </c>
+      <c r="N48">
+        <f>SMALL(B48:K48,1)</f>
+        <v>10571</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2603,8 +3787,15 @@
       <c r="J49">
         <v>28032</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="K49">
+        <v>27381</v>
+      </c>
+      <c r="N49">
+        <f>SMALL(B49:K49,1)</f>
+        <v>27381</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2635,8 +3826,15 @@
       <c r="J50">
         <v>372754</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="K50">
+        <v>270421</v>
+      </c>
+      <c r="N50">
+        <f>SMALL(B50:K50,1)</f>
+        <v>270317</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2667,8 +3865,15 @@
       <c r="J51">
         <v>270255</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="K51">
+        <v>237315</v>
+      </c>
+      <c r="N51">
+        <f>SMALL(B51:K51,1)</f>
+        <v>187174</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2699,8 +3904,317 @@
       <c r="J52">
         <v>245873</v>
       </c>
+      <c r="K52">
+        <v>188996</v>
+      </c>
+      <c r="N52">
+        <f>SMALL(B52:K52,1)</f>
+        <v>150222</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="N15:N52 B3:K3 N3:N13">
+    <cfRule type="cellIs" dxfId="69" priority="72" operator="equal">
+      <formula>$N$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:K2 N2:N3">
+    <cfRule type="cellIs" dxfId="68" priority="44" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="45" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3">
+    <cfRule type="cellIs" dxfId="66" priority="42" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="43" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4">
+    <cfRule type="cellIs" dxfId="64" priority="40" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="41" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5">
+    <cfRule type="cellIs" dxfId="62" priority="38" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="39" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6">
+    <cfRule type="cellIs" dxfId="60" priority="36" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="37" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7">
+    <cfRule type="cellIs" dxfId="58" priority="34" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="35" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8">
+    <cfRule type="cellIs" dxfId="56" priority="32" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="33" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N9">
+    <cfRule type="cellIs" dxfId="54" priority="30" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="31" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N10">
+    <cfRule type="cellIs" dxfId="52" priority="28" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="29" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N11">
+    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="27" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N12">
+    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N13">
+    <cfRule type="cellIs" dxfId="46" priority="22" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N14">
+    <cfRule type="cellIs" dxfId="44" priority="20" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15">
+    <cfRule type="cellIs" dxfId="42" priority="18" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="19" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15">
+    <cfRule type="cellIs" dxfId="40" priority="16" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16:N52">
+    <cfRule type="cellIs" dxfId="38" priority="14" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="15" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16:N52">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="13" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:K4 N4">
+    <cfRule type="cellIs" dxfId="34" priority="97" operator="equal">
+      <formula>$N$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:K5 M5:XFD5">
+    <cfRule type="cellIs" dxfId="33" priority="99" operator="equal">
+      <formula>$N$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:K6 M6:XFD6">
+    <cfRule type="cellIs" dxfId="32" priority="102" operator="equal">
+      <formula>$N$6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:K7 M7:XFD7">
+    <cfRule type="cellIs" dxfId="31" priority="105" operator="equal">
+      <formula>$N$7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:K8 M8:XFD8">
+    <cfRule type="cellIs" dxfId="30" priority="108" operator="equal">
+      <formula>$N$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:K9 M9:XFD9">
+    <cfRule type="cellIs" dxfId="29" priority="111" operator="equal">
+      <formula>$N$9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="112" operator="equal">
+      <formula>65727.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:K10 M10:XFD10">
+    <cfRule type="cellIs" dxfId="27" priority="117" operator="equal">
+      <formula>$N$10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:K11 M11:XFD11">
+    <cfRule type="cellIs" dxfId="26" priority="120" operator="equal">
+      <formula>$N$11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:K14 M14:XFD14">
+    <cfRule type="cellIs" dxfId="25" priority="145" operator="equal">
+      <formula>$N$14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:K17 M17:XFD17">
+    <cfRule type="cellIs" dxfId="24" priority="148" operator="equal">
+      <formula>$N$17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:K18 M18:XFD18">
+    <cfRule type="cellIs" dxfId="23" priority="151" operator="equal">
+      <formula>$N$18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24:K24 M24:XFD24">
+    <cfRule type="cellIs" dxfId="22" priority="154" operator="equal">
+      <formula>$N$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:K25 M25:XFD25">
+    <cfRule type="cellIs" dxfId="21" priority="157" operator="equal">
+      <formula>$N$25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:K26 M26:XFD26">
+    <cfRule type="cellIs" dxfId="20" priority="160" operator="equal">
+      <formula>$N$26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:K27 M27:XFD27">
+    <cfRule type="cellIs" dxfId="19" priority="163" operator="equal">
+      <formula>$N$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:K28 M28:XFD28">
+    <cfRule type="cellIs" dxfId="18" priority="166" operator="equal">
+      <formula>$N$28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:K29 M29:XFD29">
+    <cfRule type="cellIs" dxfId="17" priority="169" operator="equal">
+      <formula>$N$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:K31 M31:XFD31">
+    <cfRule type="cellIs" dxfId="16" priority="172" operator="equal">
+      <formula>$N$31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39:K39 M39:XFD39">
+    <cfRule type="cellIs" dxfId="15" priority="175" operator="equal">
+      <formula>$N$39</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:K41 M41:XFD41">
+    <cfRule type="cellIs" dxfId="14" priority="178" operator="equal">
+      <formula>$N$41</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:K50 M50:XFD50">
+    <cfRule type="cellIs" dxfId="13" priority="181" operator="equal">
+      <formula>$N$50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51:K51 M51:XFD51">
+    <cfRule type="cellIs" dxfId="12" priority="184" operator="equal">
+      <formula>$N$51</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52:K52 M52:XFD52">
+    <cfRule type="cellIs" dxfId="11" priority="187" operator="equal">
+      <formula>$N$52</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:N49">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>$N$49</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48:N48">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>$N$48</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47:N47">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>$N$47</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42:N42">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43:N46">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40:N40">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>$N$40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:N38">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:N30">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>$N$30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:N23">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:N16">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:N13">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added entropy values of each file
</commit_message>
<xml_diff>
--- a/Resuts/result.xlsx
+++ b/Resuts/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Filename</t>
   </si>
@@ -200,13 +200,19 @@
   </si>
   <si>
     <t>GGZRLE</t>
+  </si>
+  <si>
+    <t>Entropia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,14 +344,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -692,9 +690,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -740,7 +739,583 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="118">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1871,10 +2446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S47" sqref="S47"/>
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1882,9 +2457,10 @@
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1921,8 +2497,11 @@
       <c r="N1" t="s">
         <v>60</v>
       </c>
+      <c r="O1" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1956,12 +2535,17 @@
       <c r="K2">
         <v>12802</v>
       </c>
+      <c r="M2" s="2"/>
       <c r="N2">
-        <f>SMALL(B2:K2,1)</f>
+        <f t="shared" ref="N2:N33" si="0">SMALL(B2:K2,1)</f>
         <v>12802</v>
       </c>
+      <c r="O2">
+        <v>5.0515350000000003</v>
+      </c>
+      <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1995,12 +2579,17 @@
       <c r="K3">
         <v>266946</v>
       </c>
+      <c r="M3" s="1"/>
       <c r="N3">
-        <f>SMALL(B3:K3,1)</f>
+        <f t="shared" si="0"/>
         <v>251157</v>
       </c>
+      <c r="O3">
+        <v>4.4621079999999997</v>
+      </c>
+      <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2034,12 +2623,17 @@
       <c r="K4">
         <v>8932</v>
       </c>
+      <c r="M4" s="1"/>
       <c r="N4">
-        <f>SMALL(B4:K4,1)</f>
+        <f t="shared" si="0"/>
         <v>8932</v>
       </c>
+      <c r="O4">
+        <v>1.916836</v>
+      </c>
+      <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2073,12 +2667,17 @@
       <c r="K5">
         <v>167429</v>
       </c>
+      <c r="M5" s="1"/>
       <c r="N5">
-        <f>SMALL(B5:K5,1)</f>
+        <f t="shared" si="0"/>
         <v>160328</v>
       </c>
+      <c r="O5">
+        <v>4.446421</v>
+      </c>
+      <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2112,12 +2711,17 @@
       <c r="K6">
         <v>41241</v>
       </c>
+      <c r="M6" s="1"/>
       <c r="N6">
-        <f>SMALL(B6:K6,1)</f>
+        <f t="shared" si="0"/>
         <v>41241</v>
       </c>
+      <c r="O6">
+        <v>5.2235909999999999</v>
+      </c>
+      <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2151,12 +2755,17 @@
       <c r="K7">
         <v>173420</v>
       </c>
+      <c r="M7" s="1"/>
       <c r="N7">
-        <f>SMALL(B7:K7,1)</f>
+        <f t="shared" si="0"/>
         <v>146200</v>
       </c>
+      <c r="O7">
+        <v>7.0548979999999997</v>
+      </c>
+      <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2190,12 +2799,17 @@
       <c r="K8">
         <v>393296</v>
       </c>
+      <c r="M8" s="1"/>
       <c r="N8">
-        <f>SMALL(B8:K8,1)</f>
+        <f t="shared" si="0"/>
         <v>353514</v>
       </c>
+      <c r="O8">
+        <v>1.954647</v>
+      </c>
+      <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2231,11 +2845,15 @@
       </c>
       <c r="M9" s="1"/>
       <c r="N9">
-        <f>SMALL(B9:K9,1)</f>
+        <f t="shared" si="0"/>
         <v>14527</v>
       </c>
+      <c r="O9">
+        <v>5.3571549999999997</v>
+      </c>
+      <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2269,12 +2887,17 @@
       <c r="K10">
         <v>127720</v>
       </c>
+      <c r="M10" s="1"/>
       <c r="N10">
-        <f>SMALL(B10:K10,1)</f>
+        <f t="shared" si="0"/>
         <v>119182</v>
       </c>
+      <c r="O10">
+        <v>4.5820319999999999</v>
+      </c>
+      <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2308,12 +2931,17 @@
       <c r="K11">
         <v>179129</v>
       </c>
+      <c r="M11" s="1"/>
       <c r="N11">
-        <f>SMALL(B11:K11,1)</f>
+        <f t="shared" si="0"/>
         <v>167626</v>
       </c>
+      <c r="O11">
+        <v>4.6026439999999997</v>
+      </c>
+      <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2347,12 +2975,17 @@
       <c r="K12">
         <v>77909</v>
       </c>
+      <c r="M12" s="1"/>
       <c r="N12">
-        <f>SMALL(B12:K12,1)</f>
+        <f t="shared" si="0"/>
         <v>72718</v>
       </c>
+      <c r="O12">
+        <v>5.6463340000000004</v>
+      </c>
+      <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2386,12 +3019,17 @@
       <c r="K13">
         <v>108878</v>
       </c>
+      <c r="M13" s="1"/>
       <c r="N13">
-        <f>SMALL(B13:K13,1)</f>
+        <f t="shared" si="0"/>
         <v>101945</v>
       </c>
+      <c r="O13">
+        <v>4.4068490000000002</v>
+      </c>
+      <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2425,12 +3063,17 @@
       <c r="K14">
         <v>129331</v>
       </c>
+      <c r="M14" s="1"/>
       <c r="N14">
-        <f>SMALL(B14:K14,1)</f>
+        <f t="shared" si="0"/>
         <v>129331</v>
       </c>
+      <c r="O14">
+        <v>3.889014</v>
+      </c>
+      <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2464,12 +3107,17 @@
       <c r="K15">
         <v>22786</v>
       </c>
+      <c r="M15" s="1"/>
       <c r="N15">
-        <f>SMALL(B15:K15,1)</f>
+        <f t="shared" si="0"/>
         <v>21896</v>
       </c>
+      <c r="O15">
+        <v>5.1236790000000001</v>
+      </c>
+      <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2503,12 +3151,17 @@
       <c r="K16">
         <v>153400</v>
       </c>
+      <c r="M16" s="1"/>
       <c r="N16">
-        <f>SMALL(B16:K16,1)</f>
+        <f t="shared" si="0"/>
         <v>142748</v>
       </c>
+      <c r="O16">
+        <v>4.5209910000000004</v>
+      </c>
+      <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2542,12 +3195,17 @@
       <c r="K17">
         <v>210992</v>
       </c>
+      <c r="M17" s="1"/>
       <c r="N17">
-        <f>SMALL(B17:K17,1)</f>
+        <f t="shared" si="0"/>
         <v>210992</v>
       </c>
+      <c r="O17">
+        <v>4.3693879999999998</v>
+      </c>
+      <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2581,12 +3239,17 @@
       <c r="K18">
         <v>250200</v>
       </c>
+      <c r="M18" s="1"/>
       <c r="N18">
-        <f>SMALL(B18:K18,1)</f>
+        <f t="shared" si="0"/>
         <v>250200</v>
       </c>
+      <c r="O18">
+        <v>4.7521890000000004</v>
+      </c>
+      <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2620,12 +3283,17 @@
       <c r="K19">
         <v>196090</v>
       </c>
+      <c r="M19" s="1"/>
       <c r="N19">
-        <f>SMALL(B19:K19,1)</f>
+        <f t="shared" si="0"/>
         <v>163036</v>
       </c>
+      <c r="O19">
+        <v>7.7376569999999996</v>
+      </c>
+      <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2659,12 +3327,17 @@
       <c r="K20">
         <v>784745</v>
       </c>
+      <c r="M20" s="1"/>
       <c r="N20">
-        <f>SMALL(B20:K20,1)</f>
+        <f t="shared" si="0"/>
         <v>663477</v>
       </c>
+      <c r="O20">
+        <v>7.754956</v>
+      </c>
+      <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2698,12 +3371,17 @@
       <c r="K21">
         <v>65428</v>
       </c>
+      <c r="M21" s="1"/>
       <c r="N21">
-        <f>SMALL(B21:K21,1)</f>
+        <f t="shared" si="0"/>
         <v>52236</v>
       </c>
+      <c r="O21">
+        <v>7.4575839999999998</v>
+      </c>
+      <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2737,12 +3415,17 @@
       <c r="K22">
         <v>231366</v>
       </c>
+      <c r="M22" s="1"/>
       <c r="N22">
-        <f>SMALL(B22:K22,1)</f>
+        <f t="shared" si="0"/>
         <v>183402</v>
       </c>
+      <c r="O22">
+        <v>7.4531720000000004</v>
+      </c>
+      <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2776,12 +3459,17 @@
       <c r="K23">
         <v>62966</v>
       </c>
+      <c r="M23" s="1"/>
       <c r="N23">
-        <f>SMALL(B23:K23,1)</f>
+        <f t="shared" si="0"/>
         <v>59928</v>
       </c>
+      <c r="O23">
+        <v>4.5949749999999998</v>
+      </c>
+      <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2815,12 +3503,17 @@
       <c r="K24">
         <v>244824</v>
       </c>
+      <c r="M24" s="1"/>
       <c r="N24">
-        <f>SMALL(B24:K24,1)</f>
+        <f t="shared" si="0"/>
         <v>192368</v>
       </c>
+      <c r="O24">
+        <v>7.3005380000000004</v>
+      </c>
+      <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2854,12 +3547,17 @@
       <c r="K25">
         <v>458717</v>
       </c>
+      <c r="M25" s="1"/>
       <c r="N25">
-        <f>SMALL(B25:K25,1)</f>
+        <f t="shared" si="0"/>
         <v>411412</v>
       </c>
+      <c r="O25">
+        <v>4.5270489999999999</v>
+      </c>
+      <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2893,12 +3591,17 @@
       <c r="K26">
         <v>100494</v>
       </c>
+      <c r="M26" s="1"/>
       <c r="N26">
-        <f>SMALL(B26:K26,1)</f>
+        <f t="shared" si="0"/>
         <v>95446</v>
       </c>
+      <c r="O26">
+        <v>4.5512069999999998</v>
+      </c>
+      <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -2932,12 +3635,17 @@
       <c r="K27">
         <v>3411</v>
       </c>
+      <c r="M27" s="1"/>
       <c r="N27">
-        <f>SMALL(B27:K27,1)</f>
+        <f t="shared" si="0"/>
         <v>1783</v>
       </c>
+      <c r="O27">
+        <v>5.1234099999999998</v>
+      </c>
+      <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2971,12 +3679,17 @@
       <c r="K28">
         <v>11542</v>
       </c>
+      <c r="M28" s="1"/>
       <c r="N28">
-        <f>SMALL(B28:K28,1)</f>
+        <f t="shared" si="0"/>
         <v>10530</v>
       </c>
+      <c r="O28">
+        <v>4.6411030000000002</v>
+      </c>
+      <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3010,12 +3723,17 @@
       <c r="K29">
         <v>3740</v>
       </c>
+      <c r="M29" s="1"/>
       <c r="N29">
-        <f>SMALL(B29:K29,1)</f>
+        <f t="shared" si="0"/>
         <v>2151</v>
       </c>
+      <c r="O29">
+        <v>5.1234099999999998</v>
+      </c>
+      <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -3049,12 +3767,17 @@
       <c r="K30">
         <v>639672</v>
       </c>
+      <c r="M30" s="1"/>
       <c r="N30">
-        <f>SMALL(B30:K30,1)</f>
+        <f t="shared" si="0"/>
         <v>580327</v>
       </c>
+      <c r="O30">
+        <v>7.1114639999999998</v>
+      </c>
+      <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -3088,12 +3811,17 @@
       <c r="K31">
         <v>251310</v>
       </c>
+      <c r="M31" s="1"/>
       <c r="N31">
-        <f>SMALL(B31:K31,1)</f>
+        <f t="shared" si="0"/>
         <v>202451</v>
       </c>
+      <c r="O31">
+        <v>7.3024839999999998</v>
+      </c>
+      <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -3127,12 +3855,17 @@
       <c r="K32">
         <v>181679</v>
       </c>
+      <c r="M32" s="1"/>
       <c r="N32">
-        <f>SMALL(B32:K32,1)</f>
+        <f t="shared" si="0"/>
         <v>168170</v>
       </c>
+      <c r="O32">
+        <v>5.228618</v>
+      </c>
+      <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -3166,12 +3899,17 @@
       <c r="K33">
         <v>152334</v>
       </c>
+      <c r="M33" s="1"/>
       <c r="N33">
-        <f>SMALL(B33:K33,1)</f>
+        <f t="shared" si="0"/>
         <v>147295</v>
       </c>
+      <c r="O33">
+        <v>4.4239509999999997</v>
+      </c>
+      <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -3205,12 +3943,17 @@
       <c r="K34">
         <v>14874</v>
       </c>
+      <c r="M34" s="1"/>
       <c r="N34">
-        <f>SMALL(B34:K34,1)</f>
+        <f t="shared" ref="N34:N52" si="1">SMALL(B34:K34,1)</f>
         <v>13430</v>
       </c>
+      <c r="O34">
+        <v>5.9479879999999996</v>
+      </c>
+      <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -3244,12 +3987,17 @@
       <c r="K35">
         <v>101893</v>
       </c>
+      <c r="M35" s="1"/>
       <c r="N35">
-        <f>SMALL(B35:K35,1)</f>
+        <f t="shared" si="1"/>
         <v>93701</v>
       </c>
+      <c r="O35">
+        <v>6.260389</v>
+      </c>
+      <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3283,12 +4031,17 @@
       <c r="K36">
         <v>23025</v>
       </c>
+      <c r="M36" s="1"/>
       <c r="N36">
-        <f>SMALL(B36:K36,1)</f>
+        <f t="shared" si="1"/>
         <v>22346</v>
       </c>
+      <c r="O36">
+        <v>5.0263390000000001</v>
+      </c>
+      <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -3322,12 +4075,17 @@
       <c r="K37">
         <v>35822</v>
       </c>
+      <c r="M37" s="1"/>
       <c r="N37">
-        <f>SMALL(B37:K37,1)</f>
+        <f t="shared" si="1"/>
         <v>34370</v>
       </c>
+      <c r="O37">
+        <v>4.6514759999999997</v>
+      </c>
+      <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -3361,12 +4119,17 @@
       <c r="K38">
         <v>159881</v>
       </c>
+      <c r="M38" s="1"/>
       <c r="N38">
-        <f>SMALL(B38:K38,1)</f>
+        <f t="shared" si="1"/>
         <v>159881</v>
       </c>
+      <c r="O38">
+        <v>4.8094330000000003</v>
+      </c>
+      <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -3400,12 +4163,17 @@
       <c r="K39">
         <v>151788</v>
       </c>
+      <c r="M39" s="1"/>
       <c r="N39">
-        <f>SMALL(B39:K39,1)</f>
+        <f t="shared" si="1"/>
         <v>151788</v>
       </c>
+      <c r="O39">
+        <v>4.393942</v>
+      </c>
+      <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -3440,11 +4208,15 @@
         <v>65902</v>
       </c>
       <c r="N40">
-        <f>SMALL(B40:K40,1)</f>
+        <f t="shared" si="1"/>
         <v>65902</v>
       </c>
+      <c r="O40">
+        <v>1.2101729999999999</v>
+      </c>
+      <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -3478,12 +4250,17 @@
       <c r="K41">
         <v>240145</v>
       </c>
+      <c r="M41" s="1"/>
       <c r="N41">
-        <f>SMALL(B41:K41,1)</f>
+        <f t="shared" si="1"/>
         <v>190131</v>
       </c>
+      <c r="O41">
+        <v>7.2471800000000002</v>
+      </c>
+      <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3517,12 +4294,17 @@
       <c r="K42">
         <v>1434082</v>
       </c>
+      <c r="M42" s="1"/>
       <c r="N42">
-        <f>SMALL(B42:K42,1)</f>
+        <f t="shared" si="1"/>
         <v>1378371</v>
       </c>
+      <c r="O42">
+        <v>4.5400729999999996</v>
+      </c>
+      <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -3556,12 +4338,17 @@
       <c r="K43">
         <v>17735</v>
       </c>
+      <c r="M43" s="1"/>
       <c r="N43">
-        <f>SMALL(B43:K43,1)</f>
+        <f t="shared" si="1"/>
         <v>16772</v>
       </c>
+      <c r="O43">
+        <v>5.2353990000000001</v>
+      </c>
+      <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -3595,12 +4382,17 @@
       <c r="K44">
         <v>22717</v>
       </c>
+      <c r="M44" s="1"/>
       <c r="N44">
-        <f>SMALL(B44:K44,1)</f>
+        <f t="shared" si="1"/>
         <v>21233</v>
       </c>
+      <c r="O44">
+        <v>4.8214639999999997</v>
+      </c>
+      <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -3634,12 +4426,17 @@
       <c r="K45">
         <v>15641</v>
       </c>
+      <c r="M45" s="1"/>
       <c r="N45">
-        <f>SMALL(B45:K45,1)</f>
+        <f t="shared" si="1"/>
         <v>14820</v>
       </c>
+      <c r="O45">
+        <v>4.9167389999999997</v>
+      </c>
+      <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -3673,12 +4470,17 @@
       <c r="K46">
         <v>9186</v>
       </c>
+      <c r="M46" s="1"/>
       <c r="N46">
-        <f>SMALL(B46:K46,1)</f>
+        <f t="shared" si="1"/>
         <v>9186</v>
       </c>
+      <c r="O46">
+        <v>5.1749999999999998</v>
+      </c>
+      <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -3712,12 +4514,17 @@
       <c r="K47">
         <v>124575</v>
       </c>
+      <c r="M47" s="1"/>
       <c r="N47">
-        <f>SMALL(B47:K47,1)</f>
+        <f t="shared" si="1"/>
         <v>115899</v>
       </c>
+      <c r="O47">
+        <v>4.5003080000000004</v>
+      </c>
+      <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -3751,12 +4558,17 @@
       <c r="K48">
         <v>10571</v>
       </c>
+      <c r="M48" s="1"/>
       <c r="N48">
-        <f>SMALL(B48:K48,1)</f>
+        <f t="shared" si="1"/>
         <v>10571</v>
       </c>
+      <c r="O48">
+        <v>4.2658719999999999</v>
+      </c>
+      <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -3790,12 +4602,17 @@
       <c r="K49">
         <v>27381</v>
       </c>
+      <c r="M49" s="1"/>
       <c r="N49">
-        <f>SMALL(B49:K49,1)</f>
+        <f t="shared" si="1"/>
         <v>27381</v>
       </c>
+      <c r="O49">
+        <v>5.5327710000000003</v>
+      </c>
+      <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -3829,12 +4646,17 @@
       <c r="K50">
         <v>270421</v>
       </c>
+      <c r="M50" s="1"/>
       <c r="N50">
-        <f>SMALL(B50:K50,1)</f>
+        <f t="shared" si="1"/>
         <v>270317</v>
       </c>
+      <c r="O50">
+        <v>4.8451630000000003</v>
+      </c>
+      <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -3868,12 +4690,17 @@
       <c r="K51">
         <v>237315</v>
       </c>
+      <c r="M51" s="1"/>
       <c r="N51">
-        <f>SMALL(B51:K51,1)</f>
+        <f t="shared" si="1"/>
         <v>187174</v>
       </c>
+      <c r="O51">
+        <v>6.9582079999999999</v>
+      </c>
+      <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -3907,313 +4734,431 @@
       <c r="K52">
         <v>188996</v>
       </c>
+      <c r="M52" s="1"/>
       <c r="N52">
-        <f>SMALL(B52:K52,1)</f>
+        <f t="shared" si="1"/>
         <v>150222</v>
       </c>
+      <c r="O52">
+        <v>7.2868240000000002</v>
+      </c>
+      <c r="Q52" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="N15:N52 B3:K3 N3:N13">
-    <cfRule type="cellIs" dxfId="69" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="96" operator="equal">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:K2 N2:N3">
-    <cfRule type="cellIs" dxfId="68" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="68" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="69" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="66" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="66" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="67" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="64" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="64" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="65" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="cellIs" dxfId="62" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="62" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="63" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="60" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="60" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="61" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="cellIs" dxfId="58" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="58" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="59" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="cellIs" dxfId="56" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="56" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="57" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="54" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="54" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="55" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="52" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="52" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="53" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="50" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="51" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="48" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="49" operator="equal">
       <formula>102413</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="cellIs" dxfId="46" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="46" operator="equal">
       <formula>$N$2</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="47" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N14">
+    <cfRule type="cellIs" dxfId="92" priority="44" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="45" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15">
+    <cfRule type="cellIs" dxfId="90" priority="42" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="43" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15">
+    <cfRule type="cellIs" dxfId="88" priority="40" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="41" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16:N52">
+    <cfRule type="cellIs" dxfId="86" priority="38" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="39" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16:N52">
+    <cfRule type="cellIs" dxfId="84" priority="36" operator="equal">
+      <formula>$N$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="37" operator="equal">
+      <formula>102413</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:K4 N4">
+    <cfRule type="cellIs" dxfId="82" priority="121" operator="equal">
+      <formula>$N$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:K5 M5:N5 P5:XFD5">
+    <cfRule type="cellIs" dxfId="81" priority="123" operator="equal">
+      <formula>$N$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:K6 M6:N6 P6:XFD6">
+    <cfRule type="cellIs" dxfId="80" priority="126" operator="equal">
+      <formula>$N$6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:K7 M7:N7 P7:XFD7">
+    <cfRule type="cellIs" dxfId="79" priority="129" operator="equal">
+      <formula>$N$7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:K8 M8:N8 P8:XFD8">
+    <cfRule type="cellIs" dxfId="78" priority="132" operator="equal">
+      <formula>$N$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:K9 M9:N9 P9:XFD9">
+    <cfRule type="cellIs" dxfId="77" priority="135" operator="equal">
+      <formula>$N$9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="136" operator="equal">
+      <formula>65727.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:K10 M10:N10 P10:XFD10">
+    <cfRule type="cellIs" dxfId="75" priority="141" operator="equal">
+      <formula>$N$10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:K11 M11:N11 P11:XFD11">
+    <cfRule type="cellIs" dxfId="74" priority="144" operator="equal">
+      <formula>$N$11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:K14 M14:N14 P14:XFD14">
+    <cfRule type="cellIs" dxfId="73" priority="169" operator="equal">
+      <formula>$N$14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:K17 M17:N17 P17:XFD17">
+    <cfRule type="cellIs" dxfId="72" priority="172" operator="equal">
+      <formula>$N$17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:K18 M18:N18 P18:XFD18">
+    <cfRule type="cellIs" dxfId="71" priority="175" operator="equal">
+      <formula>$N$18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24:K24 M24:N24 P24:XFD24">
+    <cfRule type="cellIs" dxfId="70" priority="178" operator="equal">
+      <formula>$N$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:K25 M25:N25 P25:XFD25">
+    <cfRule type="cellIs" dxfId="69" priority="181" operator="equal">
+      <formula>$N$25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:K26 M26:N26 P26:XFD26">
+    <cfRule type="cellIs" dxfId="68" priority="184" operator="equal">
+      <formula>$N$26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:K27 M27:N27 P27:XFD27">
+    <cfRule type="cellIs" dxfId="67" priority="187" operator="equal">
+      <formula>$N$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:K28 M28:N28 P28:XFD28">
+    <cfRule type="cellIs" dxfId="66" priority="190" operator="equal">
+      <formula>$N$28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:K29 M29:N29 P29:XFD29">
+    <cfRule type="cellIs" dxfId="65" priority="193" operator="equal">
+      <formula>$N$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:K31 M31:N31 P31:XFD31">
+    <cfRule type="cellIs" dxfId="64" priority="196" operator="equal">
+      <formula>$N$31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39:K39 M39:N39 P39:XFD39">
+    <cfRule type="cellIs" dxfId="63" priority="199" operator="equal">
+      <formula>$N$39</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:K41 M41:N41 P41:XFD41">
+    <cfRule type="cellIs" dxfId="62" priority="202" operator="equal">
+      <formula>$N$41</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:K50 M50:N50 P50:XFD50">
+    <cfRule type="cellIs" dxfId="61" priority="205" operator="equal">
+      <formula>$N$50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51:K51 M51:N51 P51:XFD51">
+    <cfRule type="cellIs" dxfId="60" priority="208" operator="equal">
+      <formula>$N$51</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52:K52 M52:N52 P52:XFD52">
+    <cfRule type="cellIs" dxfId="59" priority="211" operator="equal">
+      <formula>$N$52</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:N49">
+    <cfRule type="cellIs" dxfId="58" priority="35" operator="equal">
+      <formula>$N$49</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48:N48">
+    <cfRule type="cellIs" dxfId="57" priority="34" operator="equal">
+      <formula>$N$48</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47:N47">
+    <cfRule type="cellIs" dxfId="56" priority="33" operator="equal">
+      <formula>$N$47</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42:N42">
+    <cfRule type="duplicateValues" dxfId="55" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43:N46">
+    <cfRule type="duplicateValues" dxfId="54" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40:N40">
+    <cfRule type="cellIs" dxfId="53" priority="30" operator="equal">
+      <formula>$N$40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:N38">
+    <cfRule type="duplicateValues" dxfId="52" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:N30">
+    <cfRule type="cellIs" dxfId="51" priority="28" operator="equal">
+      <formula>$N$30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:N23">
+    <cfRule type="duplicateValues" dxfId="50" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:N16">
+    <cfRule type="duplicateValues" dxfId="49" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:N13">
+    <cfRule type="duplicateValues" dxfId="48" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5">
     <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
-      <formula>102413</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N14">
-    <cfRule type="cellIs" dxfId="44" priority="20" operator="equal">
-      <formula>$N$2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
-      <formula>102413</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N15">
-    <cfRule type="cellIs" dxfId="42" priority="18" operator="equal">
-      <formula>$N$2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="19" operator="equal">
-      <formula>102413</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N15">
-    <cfRule type="cellIs" dxfId="40" priority="16" operator="equal">
-      <formula>$N$2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
-      <formula>102413</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N16:N52">
-    <cfRule type="cellIs" dxfId="38" priority="14" operator="equal">
-      <formula>$N$2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="15" operator="equal">
-      <formula>102413</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N16:N52">
-    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
-      <formula>$N$2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="13" operator="equal">
-      <formula>102413</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:K4 N4">
-    <cfRule type="cellIs" dxfId="34" priority="97" operator="equal">
-      <formula>$N$4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:K5 M5:XFD5">
-    <cfRule type="cellIs" dxfId="33" priority="99" operator="equal">
       <formula>$N$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:K6 M6:XFD6">
-    <cfRule type="cellIs" dxfId="32" priority="102" operator="equal">
+  <conditionalFormatting sqref="O6">
+    <cfRule type="cellIs" dxfId="43" priority="22" operator="equal">
       <formula>$N$6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:K7 M7:XFD7">
-    <cfRule type="cellIs" dxfId="31" priority="105" operator="equal">
+  <conditionalFormatting sqref="O7">
+    <cfRule type="cellIs" dxfId="41" priority="21" operator="equal">
       <formula>$N$7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:K8 M8:XFD8">
-    <cfRule type="cellIs" dxfId="30" priority="108" operator="equal">
+  <conditionalFormatting sqref="O8">
+    <cfRule type="cellIs" dxfId="39" priority="20" operator="equal">
       <formula>$N$8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:K9 M9:XFD9">
-    <cfRule type="cellIs" dxfId="29" priority="111" operator="equal">
+  <conditionalFormatting sqref="O9">
+    <cfRule type="cellIs" dxfId="37" priority="18" operator="equal">
       <formula>$N$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="19" operator="equal">
       <formula>65727.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:K10 M10:XFD10">
-    <cfRule type="cellIs" dxfId="27" priority="117" operator="equal">
+  <conditionalFormatting sqref="O10">
+    <cfRule type="cellIs" dxfId="33" priority="17" operator="equal">
       <formula>$N$10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:K11 M11:XFD11">
-    <cfRule type="cellIs" dxfId="26" priority="120" operator="equal">
+  <conditionalFormatting sqref="O11">
+    <cfRule type="cellIs" dxfId="31" priority="16" operator="equal">
       <formula>$N$11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:K14 M14:XFD14">
-    <cfRule type="cellIs" dxfId="25" priority="145" operator="equal">
+  <conditionalFormatting sqref="O14">
+    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
       <formula>$N$14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:K17 M17:XFD17">
-    <cfRule type="cellIs" dxfId="24" priority="148" operator="equal">
+  <conditionalFormatting sqref="O17">
+    <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
       <formula>$N$17</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18:K18 M18:XFD18">
-    <cfRule type="cellIs" dxfId="23" priority="151" operator="equal">
+  <conditionalFormatting sqref="O18">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
       <formula>$N$18</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A24:K24 M24:XFD24">
-    <cfRule type="cellIs" dxfId="22" priority="154" operator="equal">
+  <conditionalFormatting sqref="O24">
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
       <formula>$N$24</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A25:K25 M25:XFD25">
-    <cfRule type="cellIs" dxfId="21" priority="157" operator="equal">
+  <conditionalFormatting sqref="O25">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>$N$25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26:K26 M26:XFD26">
-    <cfRule type="cellIs" dxfId="20" priority="160" operator="equal">
+  <conditionalFormatting sqref="O26">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
       <formula>$N$26</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27:K27 M27:XFD27">
-    <cfRule type="cellIs" dxfId="19" priority="163" operator="equal">
+  <conditionalFormatting sqref="O27">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
       <formula>$N$27</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28:K28 M28:XFD28">
-    <cfRule type="cellIs" dxfId="18" priority="166" operator="equal">
+  <conditionalFormatting sqref="O28">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>$N$28</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29:K29 M29:XFD29">
-    <cfRule type="cellIs" dxfId="17" priority="169" operator="equal">
+  <conditionalFormatting sqref="O29">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>$N$29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31:K31 M31:XFD31">
-    <cfRule type="cellIs" dxfId="16" priority="172" operator="equal">
+  <conditionalFormatting sqref="O31">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>$N$31</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:K39 M39:XFD39">
-    <cfRule type="cellIs" dxfId="15" priority="175" operator="equal">
+  <conditionalFormatting sqref="O39">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>$N$39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:K41 M41:XFD41">
-    <cfRule type="cellIs" dxfId="14" priority="178" operator="equal">
+  <conditionalFormatting sqref="O41">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>$N$41</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:K50 M50:XFD50">
-    <cfRule type="cellIs" dxfId="13" priority="181" operator="equal">
+  <conditionalFormatting sqref="O50">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>$N$50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A51:K51 M51:XFD51">
-    <cfRule type="cellIs" dxfId="12" priority="184" operator="equal">
+  <conditionalFormatting sqref="O51">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>$N$51</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52:K52 M52:XFD52">
-    <cfRule type="cellIs" dxfId="11" priority="187" operator="equal">
+  <conditionalFormatting sqref="O52">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$N$52</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:N49">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
-      <formula>$N$49</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48:N48">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
-      <formula>$N$48</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47:N47">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
-      <formula>$N$47</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B42:N42">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43:N46">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40:N40">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>$N$40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32:N38">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30:N30">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>$N$30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:N23">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:N16">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:N13">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>